<commit_message>
Uren reg, scraplist edit, soundlist edit
</commit_message>
<xml_diff>
--- a/Planning/Implemented Scrap List.xlsx
+++ b/Planning/Implemented Scrap List.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162912"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="213">
   <si>
     <t>Finished + Implemented</t>
   </si>
@@ -518,12 +518,147 @@
   </si>
   <si>
     <t>6A_ Lego Attack</t>
+  </si>
+  <si>
+    <t>8SFX_DMGS_001</t>
+  </si>
+  <si>
+    <t>8SFX_DEADS_001</t>
+  </si>
+  <si>
+    <t>8SFX_KILLS_001</t>
+  </si>
+  <si>
+    <t>8SFX_EGS_001</t>
+  </si>
+  <si>
+    <t>8SFX_EAS_001</t>
+  </si>
+  <si>
+    <t>8SFX_EWS_001</t>
+  </si>
+  <si>
+    <t>8SFX_ELS_001</t>
+  </si>
+  <si>
+    <t>8SFX_AJUMPS_001</t>
+  </si>
+  <si>
+    <t>8SFX_SGLS_001</t>
+  </si>
+  <si>
+    <t>8SFX_WALKS_001</t>
+  </si>
+  <si>
+    <t>8SFX_JUMPS_001</t>
+  </si>
+  <si>
+    <t>8SFX_EWTS_001</t>
+  </si>
+  <si>
+    <t>8SFX_KTRS_001</t>
+  </si>
+  <si>
+    <t>8SFX_ATRS_001</t>
+  </si>
+  <si>
+    <t>8SFX_CTRS_001</t>
+  </si>
+  <si>
+    <t>8SFX_STRS_001</t>
+  </si>
+  <si>
+    <t>8SFX_BGM2S_001</t>
+  </si>
+  <si>
+    <t>Scrapped sfx:</t>
+  </si>
+  <si>
+    <t>8SFX_KSLAS_001</t>
+  </si>
+  <si>
+    <t>8SFX_ALSS_001</t>
+  </si>
+  <si>
+    <t>8SFX_SHITS_001</t>
+  </si>
+  <si>
+    <t>8SFX_CSHOS_001</t>
+  </si>
+  <si>
+    <t>Inplemented sfx:</t>
+  </si>
+  <si>
+    <t>8SFX_OPTS_001</t>
+  </si>
+  <si>
+    <t>8SFX_ABIS_001</t>
+  </si>
+  <si>
+    <t>8SFX_MENU_001</t>
+  </si>
+  <si>
+    <t>8SFX_BGM1_001</t>
+  </si>
+  <si>
+    <t>8SFX_BGM2_001</t>
+  </si>
+  <si>
+    <t>8SFX_BGM3_001</t>
+  </si>
+  <si>
+    <t>8SFX_DEAD_001</t>
+  </si>
+  <si>
+    <t>8SFX_HPP_001</t>
+  </si>
+  <si>
+    <t>8SFX_MANP_001</t>
+  </si>
+  <si>
+    <t>8SFX_DEAP_001</t>
+  </si>
+  <si>
+    <t>8SFX_HITP_001</t>
+  </si>
+  <si>
+    <t>8SFX_COLLP_001</t>
+  </si>
+  <si>
+    <t>8SFX_ABC_001</t>
+  </si>
+  <si>
+    <t>8SFX_KLP_001</t>
+  </si>
+  <si>
+    <t>8SFX_ADJP_001</t>
+  </si>
+  <si>
+    <t>8SFX_AHP_001</t>
+  </si>
+  <si>
+    <t>8SFX_CSHP_001</t>
+  </si>
+  <si>
+    <t>8SFX_CEXP_001</t>
+  </si>
+  <si>
+    <t>8SFX_SGP_001</t>
+  </si>
+  <si>
+    <t>8SFX_COMIC_001</t>
+  </si>
+  <si>
+    <t>8SFX_COMIC_002</t>
+  </si>
+  <si>
+    <t>8SFX_COMIC_003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -622,7 +757,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -674,7 +809,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -868,23 +1003,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N118"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="17" max="17" width="16" customWidth="1"/>
+    <col min="19" max="19" width="17.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -897,8 +1036,14 @@
       <c r="N1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="Q1" t="s">
+        <v>190</v>
+      </c>
+      <c r="S1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -911,8 +1056,14 @@
       <c r="N2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="Q2" t="s">
+        <v>186</v>
+      </c>
+      <c r="S2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -922,8 +1073,14 @@
       <c r="J3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="Q3" t="s">
+        <v>187</v>
+      </c>
+      <c r="S3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -933,8 +1090,14 @@
       <c r="J4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="Q4" t="s">
+        <v>188</v>
+      </c>
+      <c r="S4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -944,8 +1107,14 @@
       <c r="J5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="Q5" t="s">
+        <v>189</v>
+      </c>
+      <c r="S5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -955,8 +1124,14 @@
       <c r="J6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="Q6" t="s">
+        <v>191</v>
+      </c>
+      <c r="S6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -966,8 +1141,14 @@
       <c r="J7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="Q7" t="s">
+        <v>192</v>
+      </c>
+      <c r="S7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -977,8 +1158,14 @@
       <c r="J8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="Q8" t="s">
+        <v>193</v>
+      </c>
+      <c r="S8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -988,8 +1175,14 @@
       <c r="J9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="Q9" t="s">
+        <v>194</v>
+      </c>
+      <c r="S9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -999,8 +1192,14 @@
       <c r="J10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="Q10" t="s">
+        <v>195</v>
+      </c>
+      <c r="S10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1010,8 +1209,14 @@
       <c r="J11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="Q11" t="s">
+        <v>196</v>
+      </c>
+      <c r="S11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1021,8 +1226,14 @@
       <c r="J12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="Q12" t="s">
+        <v>197</v>
+      </c>
+      <c r="S12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1032,8 +1243,14 @@
       <c r="J13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="Q13" t="s">
+        <v>198</v>
+      </c>
+      <c r="S13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1043,120 +1260,180 @@
       <c r="J14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="Q14" t="s">
+        <v>199</v>
+      </c>
+      <c r="S14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
         <v>43</v>
       </c>
       <c r="J15" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="Q15" t="s">
+        <v>200</v>
+      </c>
+      <c r="S15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
         <v>45</v>
       </c>
       <c r="J16" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="Q16" t="s">
+        <v>201</v>
+      </c>
+      <c r="S16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" t="s">
         <v>47</v>
       </c>
       <c r="J17" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="Q17" t="s">
+        <v>202</v>
+      </c>
+      <c r="S17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" t="s">
         <v>49</v>
       </c>
       <c r="J18" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="Q18" t="s">
+        <v>203</v>
+      </c>
+      <c r="S18" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" t="s">
         <v>51</v>
       </c>
       <c r="J19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="Q19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" t="s">
         <v>53</v>
       </c>
       <c r="J20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="Q20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" t="s">
         <v>55</v>
       </c>
       <c r="J21" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="Q21" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" t="s">
         <v>57</v>
       </c>
       <c r="J22" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="Q22" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" t="s">
         <v>59</v>
       </c>
       <c r="J23" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="Q23" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" t="s">
         <v>61</v>
       </c>
       <c r="J24" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="Q24" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" t="s">
         <v>63</v>
       </c>
       <c r="J25" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="Q25" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" t="s">
         <v>65</v>
       </c>
       <c r="J26" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="Q26" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" t="s">
         <v>67</v>
       </c>
       <c r="J27" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="Q27" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" t="s">
         <v>69</v>
       </c>
       <c r="J28" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="Q28" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -1164,7 +1441,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:19">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -1172,7 +1449,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:19">
       <c r="A31" t="s">
         <v>75</v>
       </c>
@@ -1181,7 +1458,7 @@
       </c>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:19">
       <c r="A32" t="s">
         <v>77</v>
       </c>

</xml_diff>